<commit_message>
bdata is working properly
</commit_message>
<xml_diff>
--- a/resources/ExcelFiles/pluerat_latestfile.xlsx
+++ b/resources/ExcelFiles/pluerat_latestfile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12735" windowHeight="4980"/>
   </bookViews>
   <sheets>
     <sheet name="CloudService" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
   <externalReferences>
     <externalReference r:id="rId26"/>
   </externalReferences>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3578" uniqueCount="2311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="2311">
   <si>
     <t>Name of the Cloud Service</t>
   </si>
@@ -7862,8 +7862,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1"/>
+    <sheetView tabSelected="1" topLeftCell="G51" workbookViewId="0">
+      <selection activeCell="AI51" sqref="AI51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8100,7 +8100,9 @@
       <c r="AB2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AC2" s="4"/>
+      <c r="AC2" s="4" t="s">
+        <v>2235</v>
+      </c>
       <c r="AD2" s="4" t="s">
         <v>116</v>
       </c>
@@ -11386,7 +11388,7 @@
         <v>54</v>
       </c>
       <c r="AH32" s="4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="AI32" s="4" t="s">
         <v>2283</v>
@@ -13237,7 +13239,7 @@
         <v>54</v>
       </c>
       <c r="AH49" s="4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="AI49" s="4" t="s">
         <v>141</v>
@@ -13346,7 +13348,7 @@
         <v>54</v>
       </c>
       <c r="AH50" s="4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="AI50" s="4" t="s">
         <v>141</v>
@@ -13548,7 +13550,7 @@
         <v>54</v>
       </c>
       <c r="AH52" s="4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="AI52" s="4" t="s">
         <v>141</v>
@@ -23791,8 +23793,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23887,7 +23889,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>